<commit_message>
Wstawienie obrazów wykresów oraz ich aktualizacje i ich opisów do 1.2.4
opisy częściowo zaktualizowane
</commit_message>
<xml_diff>
--- a/pomocnicze/Wykresy pomocnicze.xlsx
+++ b/pomocnicze/Wykresy pomocnicze.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPSZ\Desktop\STUDIA\doktorat_git\pomocnicze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5850DF65-21D0-4EF3-824F-1C89E7A5F33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18155AD-5FA1-4635-B312-1887FFC97BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="833" yWindow="-98" windowWidth="23265" windowHeight="13695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2140" yWindow="-21710" windowWidth="37690" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RadarModelUniwersytetu" sheetId="1" r:id="rId1"/>
@@ -281,7 +281,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -373,7 +373,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -464,7 +464,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -576,7 +576,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -634,7 +634,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -668,7 +668,7 @@
           <c:x val="0.69998259259259266"/>
           <c:y val="0.23773624477437919"/>
           <c:w val="0.3000174074074074"/>
-          <c:h val="0.31925500000000001"/>
+          <c:h val="0.46392579363337361"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -684,7 +684,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -736,7 +736,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -765,7 +765,7 @@
           <c:x val="7.5775826819001801E-2"/>
           <c:y val="4.3117283950617286E-2"/>
           <c:w val="0.85302032471437161"/>
-          <c:h val="0.75421728395061727"/>
+          <c:h val="0.72995714790813859"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -786,7 +786,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -989,7 +989,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1427,7 +1427,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="44450" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1646,13 +1646,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="pl-PL"/>
@@ -1702,13 +1702,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="pl-PL"/>
@@ -1741,13 +1741,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="pl-PL"/>
@@ -1808,13 +1808,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="pl-PL"/>
@@ -1864,7 +1864,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -2962,15 +2962,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
+      <xdr:colOff>514348</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>125410</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>85049</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>99562</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>303448</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>141972</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3002,16 +3002,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>316705</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>19047</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>148430</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>87309</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>247405</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>1497</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>8242</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>138659</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3304,8 +3304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C6:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X38" sqref="X38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3393,7 +3393,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -3402,8 +3402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089F1355-9A40-4CDF-BFE7-020CB030EAAA}">
   <dimension ref="B3:AI37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB30" sqref="AB30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4277,7 +4277,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>